<commit_message>
ClassNotes and Midterm and Projects
</commit_message>
<xml_diff>
--- a/scooby.xlsx
+++ b/scooby.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloise/Dropbox/250 R Programming/Math 250 R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkaderbhai/MATH_250-main/MATH250/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7FA4DE6-0A1C-6044-A98B-5C71EF25EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3CD336-0446-9540-9B26-6E4AB8D840F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7225,9 +7225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7265,7 +7265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7371,7 +7371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7513,7 +7513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7523,11 +7523,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="23.5" customWidth="1"/>
+    <col min="17" max="17" width="31.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.1640625" customWidth="1"/>
+    <col min="19" max="19" width="23.83203125" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" customWidth="1"/>
+    <col min="21" max="21" width="30.5" customWidth="1"/>
+    <col min="22" max="22" width="27.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" customWidth="1"/>
+    <col min="24" max="24" width="16.5" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="15.5" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.1640625" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" customWidth="1"/>
+    <col min="30" max="30" width="14.6640625" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" customWidth="1"/>
+    <col min="32" max="32" width="15.1640625" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" customWidth="1"/>
+    <col min="34" max="34" width="13.5" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>